<commit_message>
Updated locality and fishing gear
Cross referenced locality, fishing gear, and date with the NMNH collection library.
</commit_message>
<xml_diff>
--- a/Data/Albatross_LWR_data/Calculated_variables.xlsx
+++ b/Data/Albatross_LWR_data/Calculated_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabes\Documents\AlbatrossPhillipinesLWR\Data\Albatross_LWR_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BBAC1A-2D77-4284-ABD2-CDD1194D10B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720B155-D4B2-440C-A11E-36727637A2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="90" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="132">
   <si>
     <t>Species</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Glossogobius_giuris</t>
   </si>
   <si>
-    <t>Naujan, Mindoro</t>
-  </si>
-  <si>
     <t>05_June_08</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>19_Jan_08</t>
   </si>
   <si>
-    <t>250_ft_seine</t>
-  </si>
-  <si>
     <t>Palawan_stream_near_Chase_Head_village</t>
   </si>
   <si>
@@ -323,15 +317,9 @@
     <t>21_Apr_08</t>
   </si>
   <si>
-    <t>Port_Busan_Busuanga_Island</t>
-  </si>
-  <si>
     <t>17_Dec_08</t>
   </si>
   <si>
-    <t>unkown</t>
-  </si>
-  <si>
     <t>Bolinao_Bay_Luzon</t>
   </si>
   <si>
@@ -408,6 +396,42 @@
   </si>
   <si>
     <t>No reported LWR on Fishbase</t>
+  </si>
+  <si>
+    <t>Naujan_Mindoro</t>
+  </si>
+  <si>
+    <t>23_Apr_08</t>
+  </si>
+  <si>
+    <t>Linacapan_Island_Burias</t>
+  </si>
+  <si>
+    <t>19_Dec_08</t>
+  </si>
+  <si>
+    <t>Port_Uson_Busuanga_Island</t>
+  </si>
+  <si>
+    <t>Dipnet_Electric_Light</t>
+  </si>
+  <si>
+    <t>Seine</t>
+  </si>
+  <si>
+    <t>250_ftm_seine</t>
+  </si>
+  <si>
+    <t>Dynamite_25_ft_seine</t>
+  </si>
+  <si>
+    <t>Dynamite_16_ft_45_ft_seine</t>
+  </si>
+  <si>
+    <t>150_ft_shore_seine</t>
+  </si>
+  <si>
+    <t>8_May_08</t>
   </si>
 </sst>
 </file>
@@ -831,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S50" sqref="S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -854,46 +878,46 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>122</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>6</v>
@@ -986,8 +1010,8 @@
       <c r="T3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="4" t="s">
-        <v>13</v>
+      <c r="U3" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -1065,6 +1089,9 @@
       <c r="S5" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="T5" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="U5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1104,13 +1131,13 @@
         <v>150</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="U6" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1145,13 +1172,13 @@
         <v>145.1</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U7" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1186,13 +1213,13 @@
         <v>147.6</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U8" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1227,10 +1254,10 @@
         <v>233</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U9" t="s">
         <v>13</v>
@@ -1244,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10" s="8">
         <v>1.873E-2</v>
@@ -1271,7 +1298,7 @@
         <v>1.7365409999999999</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M10" s="9">
         <v>0.09</v>
@@ -1330,7 +1357,7 @@
         <v>24</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -1412,7 +1439,7 @@
         <v>28</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="8" customFormat="1">
@@ -1423,7 +1450,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="8">
         <v>1.193E-2</v>
@@ -1450,7 +1477,7 @@
         <v>2.162706</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M14" s="9">
         <v>2.7639999999999998</v>
@@ -1503,13 +1530,13 @@
         <v>115</v>
       </c>
       <c r="S15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="T15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T15" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="U15" s="4" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1544,13 +1571,13 @@
         <v>64.099999999999994</v>
       </c>
       <c r="S16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T16" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="U16" s="4" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -1585,13 +1612,13 @@
         <v>75.900000000000006</v>
       </c>
       <c r="S17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T17" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="U17" s="4" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:22" s="8" customFormat="1">
@@ -1602,7 +1629,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" s="8">
         <v>8.7360000000000007E-3</v>
@@ -1629,7 +1656,7 @@
         <v>1.281498</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M18" s="9">
         <v>0.10299999999999999</v>
@@ -1652,7 +1679,7 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3">
         <v>4</v>
@@ -1682,24 +1709,24 @@
         <v>65.900000000000006</v>
       </c>
       <c r="S19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="T19" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="U19" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L20" s="3">
         <v>25</v>
@@ -1723,24 +1750,24 @@
         <v>93.1</v>
       </c>
       <c r="S20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T20" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="U20" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="8" customFormat="1">
       <c r="A21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="9">
         <v>4</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="8">
         <v>2.4577000000000002E-3</v>
@@ -1767,7 +1794,7 @@
         <v>0.4383185</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M21" s="9">
         <v>0.25900000000000001</v>
@@ -1790,7 +1817,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="3">
         <v>5</v>
@@ -1820,24 +1847,24 @@
         <v>76.8</v>
       </c>
       <c r="S22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T22" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="U22" s="4" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="8" customFormat="1">
       <c r="A23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="8">
         <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" s="8">
         <v>2.3411999999999999E-2</v>
@@ -1864,7 +1891,7 @@
         <v>2.274273</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M23" s="9">
         <v>1.423</v>
@@ -1887,7 +1914,7 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" s="3">
         <v>6</v>
@@ -1917,10 +1944,10 @@
         <v>80</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U24" s="4" t="s">
         <v>13</v>
@@ -1928,7 +1955,7 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" s="3">
         <v>6</v>
@@ -1958,25 +1985,25 @@
         <v>96.9</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="V25" s="3"/>
     </row>
     <row r="26" spans="1:22" s="8" customFormat="1">
       <c r="A26" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="9">
         <v>6</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="8">
         <v>3.1066E-2</v>
@@ -2003,7 +2030,7 @@
         <v>2.538351</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M26" s="9">
         <v>0.111</v>
@@ -2029,7 +2056,7 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3">
         <v>7</v>
@@ -2059,10 +2086,10 @@
         <v>119.7</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U27" s="4" t="s">
         <v>13</v>
@@ -2070,13 +2097,13 @@
     </row>
     <row r="28" spans="1:22" s="8" customFormat="1">
       <c r="A28" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" s="9">
         <v>7</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28" s="8">
         <v>1.2192E-2</v>
@@ -2103,7 +2130,7 @@
         <v>1.843529</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M28" s="9">
         <v>0.29880000000000001</v>
@@ -2126,7 +2153,7 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29" s="3">
         <v>8</v>
@@ -2156,18 +2183,18 @@
         <v>63.5</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B30" s="3">
         <v>8</v>
@@ -2197,18 +2224,18 @@
         <v>59</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U30" s="4" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B31" s="7">
         <v>8</v>
@@ -2238,18 +2265,18 @@
         <v>27.9</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" s="7">
         <v>8</v>
@@ -2279,24 +2306,24 @@
         <v>62</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U32" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:22" s="8" customFormat="1">
       <c r="A33" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B33" s="10">
         <v>8</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D33" s="11">
         <v>7.9120000000000006E-3</v>
@@ -2323,7 +2350,7 @@
         <v>0.95143739999999999</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M33" s="9">
         <v>4.2000000000000003E-2</v>
@@ -2346,7 +2373,7 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="3">
         <v>9</v>
@@ -2376,18 +2403,18 @@
         <v>67.3</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" s="7">
         <v>9</v>
@@ -2417,24 +2444,24 @@
         <v>44.2</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:22" s="8" customFormat="1">
       <c r="A36" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="10">
         <v>9</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D36" s="11">
         <v>5.9858000000000003E-3</v>
@@ -2461,7 +2488,7 @@
         <v>0.74989059999999996</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M36" s="9">
         <v>0.08</v>
@@ -2484,7 +2511,7 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" s="7">
         <v>10</v>
@@ -2514,10 +2541,10 @@
         <v>103.7</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="U37" s="4" t="s">
         <v>13</v>
@@ -2525,7 +2552,7 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="7">
         <v>10</v>
@@ -2555,24 +2582,24 @@
         <v>80.599999999999994</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="T38" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="U38" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="15" customFormat="1">
       <c r="A39" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B39" s="14">
         <v>10</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D39" s="15">
         <v>1.9105E-2</v>
@@ -2599,7 +2626,7 @@
         <v>1.0479259999999999</v>
       </c>
       <c r="L39" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M39" s="15">
         <v>4.4200000000000003E-2</v>
@@ -2622,7 +2649,7 @@
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B40" s="7">
         <v>11</v>
@@ -2637,33 +2664,33 @@
         <v>2.548</v>
       </c>
       <c r="N40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O40">
         <v>50.2</v>
       </c>
       <c r="P40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q40">
         <v>62</v>
       </c>
       <c r="R40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="U40" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B41" s="7">
         <v>11</v>
@@ -2693,18 +2720,18 @@
         <v>44.3</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U41" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:22">
       <c r="A42" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B42" s="7">
         <v>11</v>
@@ -2734,24 +2761,24 @@
         <v>27.8</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="U42" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="15" customFormat="1">
       <c r="A43" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B43" s="15">
         <v>11</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43" s="15">
         <v>1.4976400000000001E-2</v>
@@ -2778,7 +2805,7 @@
         <v>1.6989240000000001</v>
       </c>
       <c r="L43" s="15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M43" s="15">
         <v>9.5000000000000001E-2</v>
@@ -2799,12 +2826,12 @@
         <v>62</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B44" s="7">
         <v>12</v>
@@ -2834,10 +2861,10 @@
         <v>64.5</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="U44" t="s">
         <v>13</v>
@@ -2845,7 +2872,7 @@
     </row>
     <row r="45" spans="1:22" s="17" customFormat="1">
       <c r="A45" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B45" s="16">
         <v>12</v>
@@ -2875,18 +2902,18 @@
         <v>58.3</v>
       </c>
       <c r="S45" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="T45" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="U45" s="17" t="s">
-        <v>13</v>
+        <v>99</v>
+      </c>
+      <c r="U45" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:22">
       <c r="A46" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B46" s="7">
         <v>12</v>
@@ -2927,7 +2954,7 @@
     </row>
     <row r="47" spans="1:22">
       <c r="A47" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B47" s="7">
         <v>12</v>
@@ -2957,18 +2984,18 @@
         <v>60.1</v>
       </c>
       <c r="S47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="T47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="U47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:22">
       <c r="A48" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B48" s="7">
         <v>12</v>
@@ -2998,24 +3025,24 @@
         <v>83.6</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="T48" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="U48" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:22" s="15" customFormat="1">
       <c r="A49" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B49" s="14">
         <v>12</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D49" s="15">
         <v>9.7447999999999996E-3</v>
@@ -3042,7 +3069,7 @@
         <v>1.281498</v>
       </c>
       <c r="L49" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M49" s="15">
         <v>8.5999999999999993E-2</v>
@@ -3065,7 +3092,7 @@
     </row>
     <row r="50" spans="1:22">
       <c r="A50" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B50" s="7">
         <v>13</v>
@@ -3094,10 +3121,19 @@
       <c r="R50">
         <v>59</v>
       </c>
+      <c r="S50" t="s">
+        <v>23</v>
+      </c>
+      <c r="T50" t="s">
+        <v>24</v>
+      </c>
+      <c r="U50" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="51" spans="1:22">
       <c r="A51" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B51" s="7">
         <v>13</v>
@@ -3126,10 +3162,19 @@
       <c r="R51">
         <v>96.1</v>
       </c>
+      <c r="S51" t="s">
+        <v>96</v>
+      </c>
+      <c r="T51" t="s">
+        <v>121</v>
+      </c>
+      <c r="U51" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="52" spans="1:22">
       <c r="A52" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B52">
         <v>13</v>
@@ -3158,16 +3203,25 @@
       <c r="R52">
         <v>67.099999999999994</v>
       </c>
+      <c r="S52" t="s">
+        <v>122</v>
+      </c>
+      <c r="T52" t="s">
+        <v>123</v>
+      </c>
+      <c r="U52" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="53" spans="1:22" s="8" customFormat="1">
       <c r="A53" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B53" s="8">
         <v>13</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D53" s="8">
         <v>5.9858999999999997E-3</v>
@@ -3194,7 +3248,7 @@
         <v>1.368512</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M53" s="8">
         <v>0.11799999999999999</v>
@@ -3215,7 +3269,7 @@
         <v>96.1</v>
       </c>
       <c r="V53" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>